<commit_message>
Implement safe flag mechanism for Eps and Telecom
</commit_message>
<xml_diff>
--- a/docs/parameters.xlsx
+++ b/docs/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildesimoni/Desktop/EPFL/sem3/semester_project/digital_twin_CubeSat/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272787B8-741E-F343-85DA-FCB5C56B1BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02ACD25-A918-6848-A68B-F32D6068872A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>Mission</t>
   </si>
@@ -515,6 +515,18 @@
   <si>
     <t>Data generated all the time: 2.5 KB = 20 Kb = 0.02 Mb / 5 min (not continuous)
 If implemented as “continuous”: 6.67e-5 Mbps</t>
+  </si>
+  <si>
+    <t>Max Time Without Communication</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>This value is the upper bound for the time without communication and will raise a safe flag (which means going to safe mode) if reached</t>
+  </si>
+  <si>
+    <t>Random, not provided by the team yet</t>
   </si>
 </sst>
 </file>
@@ -662,7 +674,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -811,12 +823,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -917,21 +966,21 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -961,6 +1010,15 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1305,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E9D23A-53C3-4A49-8E10-F5E4A83E23C6}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1317,107 +1375,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="46"/>
+      <c r="A1" s="44"/>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
     </row>
     <row r="2" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="45"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+      <c r="A3" s="44"/>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="45"/>
       <c r="C4" s="45"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="48" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="45"/>
       <c r="C5" s="45"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="48" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="47" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="50" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="50" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="47" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="44">
+      <c r="A14" s="49">
         <v>45611</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="44"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A12:C12"/>
@@ -1428,6 +1481,11 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2163,10 +2221,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231E77F-1773-2E41-B790-1227F4645A90}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2418,6 +2476,23 @@
       </c>
       <c r="E16" s="32" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B17" s="61">
+        <v>1</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change parameters and check propagation with different timesteps
</commit_message>
<xml_diff>
--- a/docs/parameters.xlsx
+++ b/docs/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildesimoni/Desktop/EPFL/sem3/semester_project/digital_twin_CubeSat/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C5739A-3A5B-BB43-BCBA-EA7886F87B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326504D3-685B-AC43-AEEF-2CEC5D69FC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="142">
   <si>
     <t>Mission</t>
   </si>
@@ -539,32 +539,86 @@
     <t>Sun spin</t>
   </si>
   <si>
-    <t>Magnetic spin</t>
-  </si>
-  <si>
-    <t>Sun pointing</t>
-  </si>
-  <si>
-    <t>Ground pointing</t>
-  </si>
-  <si>
-    <t>Prograde pointing</t>
-  </si>
-  <si>
-    <t>Z+ towards sun</t>
-  </si>
-  <si>
     <t>Z- towards GS</t>
   </si>
   <si>
     <t>Z- towards nadir (Earth's surface)</t>
+  </si>
+  <si>
+    <t>Y/Z Thomson spin</t>
+  </si>
+  <si>
+    <t>Nadir pointing</t>
+  </si>
+  <si>
+    <t>Nadir spin</t>
+  </si>
+  <si>
+    <t>Ground tracking</t>
+  </si>
+  <si>
+    <t>Z+ towards sun + can rotate along Z axis *</t>
+  </si>
+  <si>
+    <t>Z- towards nadir (Earth's surface) + can rotate along Z axis *</t>
+  </si>
+  <si>
+    <t>Satellite rotates along inertia axes. Enable to passively stabilize the satellite without consuming too much energy. Commonly used during eclipses.</t>
+  </si>
+  <si>
+    <t>* : the spin is so that ADCS's reaction wheels don't need to be used (they consumne a lot of energy)</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: SMA</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: ECC</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: INC</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: AOP</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: RAAN</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: TA</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>MDD</t>
+  </si>
+  <si>
+    <t>Chosen so that the altitude is 500km</t>
+  </si>
+  <si>
+    <t>Random for now.</t>
+  </si>
+  <si>
+    <t>Based on the chosen SMA and the ECC, this is the only value that allows for a sun-synchronous orbit</t>
+  </si>
+  <si>
+    <t>Circular orbit</t>
+  </si>
+  <si>
+    <t>Lausanne GS: latitude</t>
+  </si>
+  <si>
+    <t>Lausanne GS: longitude</t>
+  </si>
+  <si>
+    <t>Lausanne GS: min elevation angle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -679,6 +733,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -718,7 +778,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -922,12 +982,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1043,63 +1183,11 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="11" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1107,6 +1195,106 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1116,8 +1304,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFE2EFDA"/>
       <color rgb="FFA8D08D"/>
-      <color rgb="FFE2EFDA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1462,99 +1650,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="51"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
+      <c r="A1" s="64"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
     </row>
     <row r="2" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="51"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
+      <c r="A3" s="64"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="63"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A7" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="53" t="s">
+      <c r="A10" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="50"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="63"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="63"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="52" t="s">
+      <c r="A12" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="63"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="49">
+      <c r="A14" s="62">
         <v>45611</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="64"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -1580,10 +1768,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D47EFD6-0811-8141-81C1-0849D4B1537E}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1596,20 +1784,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1659,26 +1847,217 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="170" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="82" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="30">
+      <c r="B6" s="83">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="E6" s="43"/>
+      <c r="E6" s="84"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="86">
+        <v>6878</v>
+      </c>
+      <c r="C7" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="87" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="89">
+        <v>0</v>
+      </c>
+      <c r="C8" s="89"/>
+      <c r="D8" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="90"/>
+    </row>
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="89">
+        <v>97.406499999999994</v>
+      </c>
+      <c r="C9" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="89" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="90"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B10" s="89">
+        <v>0</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" s="90"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="88" t="s">
+        <v>131</v>
+      </c>
+      <c r="B11" s="89">
+        <v>110</v>
+      </c>
+      <c r="C11" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="E11" s="90"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" s="92">
+        <v>0</v>
+      </c>
+      <c r="C12" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="92" t="s">
+        <v>136</v>
+      </c>
+      <c r="E12" s="93"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="85" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="86">
+        <v>46.52</v>
+      </c>
+      <c r="C13" s="86" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="86"/>
+      <c r="E13" s="94" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="88" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="89">
+        <v>6.5650000000000004</v>
+      </c>
+      <c r="C14" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="89"/>
+      <c r="E14" s="95"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="91" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="92">
+        <v>10</v>
+      </c>
+      <c r="C15" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="92"/>
+      <c r="E15" s="96"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="81"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="81"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="81"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="81"/>
+      <c r="E17" s="81"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="81"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="81"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="81"/>
+      <c r="D19" s="81"/>
+      <c r="E19" s="81"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="81"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
+      <c r="D20" s="81"/>
+      <c r="E20" s="81"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="81"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="81"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="81"/>
+      <c r="D22" s="81"/>
+      <c r="E22" s="81"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="81"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="81"/>
+      <c r="D23" s="81"/>
+      <c r="E23" s="81"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:E2"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="E13:E15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" location="gid=0" xr:uid="{1DD03B05-28A9-644D-B97F-B9541B9F25FF}"/>
+    <hyperlink ref="E7:E12" r:id="rId2" display="MDD" xr:uid="{84FB9A2A-1652-1540-B749-67CDF3108C37}"/>
+    <hyperlink ref="E13:E15" r:id="rId3" display="MDD" xr:uid="{0E5E460C-7545-BB44-8B3F-8FDC28BF388A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1688,7 +2067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11073C-47B1-364A-8420-1F44036F49B1}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="94" workbookViewId="0">
+    <sheetView zoomScale="94" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1702,20 +2081,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="69" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1941,16 +2320,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
       <c r="I1" s="9" t="s">
         <v>61</v>
       </c>
@@ -1959,14 +2338,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="11" t="s">
         <v>63</v>
       </c>
@@ -1975,28 +2354,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="71" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="58"/>
-      <c r="B4" s="58"/>
+      <c r="A4" s="71"/>
+      <c r="B4" s="71"/>
       <c r="C4" s="6" t="s">
         <v>47</v>
       </c>
@@ -2215,10 +2594,10 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="59"/>
+      <c r="B12" s="72"/>
       <c r="C12" s="40">
         <v>6.25</v>
       </c>
@@ -2310,7 +2689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1231E77F-1773-2E41-B790-1227F4645A90}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="125" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -2324,20 +2703,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="56"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -2357,16 +2736,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="77" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="62">
+      <c r="B4" s="75">
         <v>0.111</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="60" t="s">
+      <c r="D4" s="73" t="s">
         <v>107</v>
       </c>
       <c r="E4" s="21" t="s">
@@ -2374,10 +2753,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
+      <c r="A5" s="78"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
       <c r="E5" s="25" t="s">
         <v>70</v>
       </c>
@@ -2611,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5DEFD8-04BD-5D41-9D2E-67579D0C1A1E}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2623,11 +3002,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
@@ -2639,140 +3018,118 @@
       <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="75" t="s">
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+    </row>
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="51"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="53" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C4" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="49"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="75" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="72" t="s">
+      <c r="C6" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="53" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="C4" s="74" t="s">
-        <v>121</v>
-      </c>
-      <c r="D4" s="66"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="72" t="s">
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="55" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="C8" s="58" t="s">
         <v>118</v>
       </c>
-      <c r="C5" s="74" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="72" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="D6" s="66"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="66"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="66"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="72" t="s">
-        <v>119</v>
-      </c>
-      <c r="C7" s="74" t="s">
-        <v>122</v>
-      </c>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
-        <v>115</v>
-      </c>
-      <c r="B8" s="77" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="79"/>
+      <c r="D8" s="59"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="76"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="73"/>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="73"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="73"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="73"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="73"/>
-      <c r="B17" s="73"/>
-      <c r="C17" s="73"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="69"/>
+      <c r="A9" s="56"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="61" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
save state to start back from simulation
</commit_message>
<xml_diff>
--- a/docs/parameters.xlsx
+++ b/docs/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildesimoni/Desktop/EPFL/sem3/semester_project/digital_twin_CubeSat/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{326504D3-685B-AC43-AEEF-2CEC5D69FC9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F9DA0A-ECC4-B248-B007-ED4EE71E9B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -408,9 +408,117 @@
     </r>
   </si>
   <si>
+    <t>Data generated during measurement mode only. A measurement window lasts 176 min (10560 s) but data is measured during 120 min only
+Calculations: 120 min of measurement generates 100MB = 800 Mb
+=&gt; the TOF measure rate should be 800/(120*60) = 0.111 Mbps</t>
+  </si>
+  <si>
+    <t>Data generated all the time except in Safe mode. Based on the SE_DSD, 29.25MB = 234Mb is generated in 10 hours. So the GNSS rate should be 234/(10*60*60) = 0.0065 Mbps</t>
+  </si>
+  <si>
+    <t>Data generated all the time: 2.5 KB = 20 Kb = 0.02 Mb / 5 min (not continuous)
+If implemented as “continuous”: 6.67e-5 Mbps</t>
+  </si>
+  <si>
+    <t>Max Time Without Communication</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>This value is the upper bound for the time without communication and will raise a safe flag (which means going to safe mode) if reached</t>
+  </si>
+  <si>
+    <t>Random, not provided by the team yet</t>
+  </si>
+  <si>
+    <t>Attitude</t>
+  </si>
+  <si>
+    <t>MEASUREMEMNT</t>
+  </si>
+  <si>
+    <t>Sun spin</t>
+  </si>
+  <si>
+    <t>Z- towards GS</t>
+  </si>
+  <si>
+    <t>Z- towards nadir (Earth's surface)</t>
+  </si>
+  <si>
+    <t>Y/Z Thomson spin</t>
+  </si>
+  <si>
+    <t>Nadir pointing</t>
+  </si>
+  <si>
+    <t>Nadir spin</t>
+  </si>
+  <si>
+    <t>Ground tracking</t>
+  </si>
+  <si>
+    <t>Z+ towards sun + can rotate along Z axis *</t>
+  </si>
+  <si>
+    <t>Z- towards nadir (Earth's surface) + can rotate along Z axis *</t>
+  </si>
+  <si>
+    <t>Satellite rotates along inertia axes. Enable to passively stabilize the satellite without consuming too much energy. Commonly used during eclipses.</t>
+  </si>
+  <si>
+    <t>* : the spin is so that ADCS's reaction wheels don't need to be used (they consumne a lot of energy)</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: SMA</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: ECC</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: INC</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: AOP</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: RAAN</t>
+  </si>
+  <si>
+    <t>Baseline Orbit: TA</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>MDD</t>
+  </si>
+  <si>
+    <t>Chosen so that the altitude is 500km</t>
+  </si>
+  <si>
+    <t>Random for now.</t>
+  </si>
+  <si>
+    <t>Based on the chosen SMA and the ECC, this is the only value that allows for a sun-synchronous orbit</t>
+  </si>
+  <si>
+    <t>Circular orbit</t>
+  </si>
+  <si>
+    <t>Lausanne GS: latitude</t>
+  </si>
+  <si>
+    <t>Lausanne GS: longitude</t>
+  </si>
+  <si>
+    <t>Lausanne GS: min elevation angle</t>
+  </si>
+  <si>
     <r>
-      <t>Average cross section used to compute drag forces in the propagation. Later, will be replaced when ADCS module with attitude change is implemented
-Calculations: 
+      <t>Average cross section used to compute drag forces in the propagation.
+Initial Calculations: 
 - solar panels dimensions: 83mm * 325mm * 2.5 mm
 - face area of 4 solar panels: 0.1079 m</t>
     </r>
@@ -502,116 +610,38 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
+      <t xml:space="preserve">2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+However, we later decided to use a cross section calculate with the DRAMA software (tool named CROC for CROss section of Complex Bodies). The obtained result (0.084 m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <t>Data generated during measurement mode only. A measurement window lasts 176 min (10560 s) but data is measured during 120 min only
-Calculations: 120 min of measurement generates 100MB = 800 Mb
-=&gt; the TOF measure rate should be 800/(120*60) = 0.111 Mbps</t>
-  </si>
-  <si>
-    <t>Data generated all the time except in Safe mode. Based on the SE_DSD, 29.25MB = 234Mb is generated in 10 hours. So the GNSS rate should be 234/(10*60*60) = 0.0065 Mbps</t>
-  </si>
-  <si>
-    <t>Data generated all the time: 2.5 KB = 20 Kb = 0.02 Mb / 5 min (not continuous)
-If implemented as “continuous”: 6.67e-5 Mbps</t>
-  </si>
-  <si>
-    <t>Max Time Without Communication</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>This value is the upper bound for the time without communication and will raise a safe flag (which means going to safe mode) if reached</t>
-  </si>
-  <si>
-    <t>Random, not provided by the team yet</t>
-  </si>
-  <si>
-    <t>Attitude</t>
-  </si>
-  <si>
-    <t>MEASUREMEMNT</t>
-  </si>
-  <si>
-    <t>Sun spin</t>
-  </si>
-  <si>
-    <t>Z- towards GS</t>
-  </si>
-  <si>
-    <t>Z- towards nadir (Earth's surface)</t>
-  </si>
-  <si>
-    <t>Y/Z Thomson spin</t>
-  </si>
-  <si>
-    <t>Nadir pointing</t>
-  </si>
-  <si>
-    <t>Nadir spin</t>
-  </si>
-  <si>
-    <t>Ground tracking</t>
-  </si>
-  <si>
-    <t>Z+ towards sun + can rotate along Z axis *</t>
-  </si>
-  <si>
-    <t>Z- towards nadir (Earth's surface) + can rotate along Z axis *</t>
-  </si>
-  <si>
-    <t>Satellite rotates along inertia axes. Enable to passively stabilize the satellite without consuming too much energy. Commonly used during eclipses.</t>
-  </si>
-  <si>
-    <t>* : the spin is so that ADCS's reaction wheels don't need to be used (they consumne a lot of energy)</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: SMA</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: ECC</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: INC</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: AOP</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: RAAN</t>
-  </si>
-  <si>
-    <t>Baseline Orbit: TA</t>
-  </si>
-  <si>
-    <t>km</t>
-  </si>
-  <si>
-    <t>MDD</t>
-  </si>
-  <si>
-    <t>Chosen so that the altitude is 500km</t>
-  </si>
-  <si>
-    <t>Random for now.</t>
-  </si>
-  <si>
-    <t>Based on the chosen SMA and the ECC, this is the only value that allows for a sun-synchronous orbit</t>
-  </si>
-  <si>
-    <t>Circular orbit</t>
-  </si>
-  <si>
-    <t>Lausanne GS: latitude</t>
-  </si>
-  <si>
-    <t>Lausanne GS: longitude</t>
-  </si>
-  <si>
-    <t>Lausanne GS: min elevation angle</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>) simulates a "randomly tumbling" satellite.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1196,27 +1226,75 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1246,54 +1324,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="24" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1650,107 +1680,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="64"/>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
+      <c r="A1" s="72"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
     </row>
     <row r="2" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="64"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
+      <c r="A3" s="72"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="64"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
+      <c r="A6" s="72"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="67" t="s">
+      <c r="A8" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="62">
+      <c r="A14" s="77">
         <v>45611</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="64"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A12:C12"/>
@@ -1761,6 +1786,11 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1770,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D47EFD6-0811-8141-81C1-0849D4B1537E}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,20 +1814,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="79" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -1846,207 +1876,207 @@
         <v>103</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="170" x14ac:dyDescent="0.2">
-      <c r="A6" s="82" t="s">
+    <row r="6" spans="1:5" ht="220" x14ac:dyDescent="0.2">
+      <c r="A6" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="B6" s="83">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C6" s="83" t="s">
+      <c r="B6" s="64">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C6" s="64" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="83" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="84"/>
+      <c r="D6" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="65"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="85" t="s">
+      <c r="A7" s="66" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="67">
+        <v>6878</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="81" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="86">
-        <v>6878</v>
-      </c>
-      <c r="C7" s="86" t="s">
+      <c r="B8" s="69">
+        <v>0</v>
+      </c>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69" t="s">
+        <v>137</v>
+      </c>
+      <c r="E8" s="82"/>
+    </row>
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B9" s="69">
+        <v>97.406499999999994</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>136</v>
+      </c>
+      <c r="E9" s="82"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="69">
+        <v>0</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="82"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="69">
+        <v>110</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" s="82"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="70" t="s">
+        <v>131</v>
+      </c>
+      <c r="B12" s="71">
+        <v>0</v>
+      </c>
+      <c r="C12" s="71" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" s="83"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="66" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="67">
+        <v>46.52</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="67"/>
+      <c r="E13" s="84" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="86" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="87" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="88" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="89">
-        <v>0</v>
-      </c>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="90"/>
-    </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="88" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="89">
-        <v>97.406499999999994</v>
-      </c>
-      <c r="C9" s="89" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="69">
+        <v>6.5650000000000004</v>
+      </c>
+      <c r="C14" s="69" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="89" t="s">
-        <v>137</v>
-      </c>
-      <c r="E9" s="90"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="88" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="89">
-        <v>0</v>
-      </c>
-      <c r="C10" s="89" t="s">
+      <c r="D14" s="69"/>
+      <c r="E14" s="85"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" s="71">
+        <v>10</v>
+      </c>
+      <c r="C15" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="89" t="s">
-        <v>136</v>
-      </c>
-      <c r="E10" s="90"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="88" t="s">
-        <v>131</v>
-      </c>
-      <c r="B11" s="89">
-        <v>110</v>
-      </c>
-      <c r="C11" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="89" t="s">
-        <v>136</v>
-      </c>
-      <c r="E11" s="90"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="91" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="92">
-        <v>0</v>
-      </c>
-      <c r="C12" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="92" t="s">
-        <v>136</v>
-      </c>
-      <c r="E12" s="93"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="85" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="86">
-        <v>46.52</v>
-      </c>
-      <c r="C13" s="86" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="94" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="89">
-        <v>6.5650000000000004</v>
-      </c>
-      <c r="C14" s="89" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="95"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="91" t="s">
-        <v>141</v>
-      </c>
-      <c r="B15" s="92">
-        <v>10</v>
-      </c>
-      <c r="C15" s="92" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="96"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="86"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
+      <c r="A16" s="62"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="62"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="81"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
+      <c r="A17" s="62"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="81"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="62"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="81"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
+      <c r="A19" s="62"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="81"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="81"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="81"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="A21" s="62"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="81"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="81"/>
-      <c r="D22" s="81"/>
-      <c r="E22" s="81"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="81"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
+      <c r="A23" s="62"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2081,20 +2111,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -2320,16 +2350,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="79" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="9" t="s">
         <v>61</v>
       </c>
@@ -2338,14 +2368,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="I2" s="11" t="s">
         <v>63</v>
       </c>
@@ -2354,28 +2384,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="71" t="s">
+      <c r="C3" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
-      <c r="B4" s="71"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
       <c r="C4" s="6" t="s">
         <v>47</v>
       </c>
@@ -2594,10 +2624,10 @@
       <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="72"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="40">
         <v>6.25</v>
       </c>
@@ -2703,20 +2733,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -2736,27 +2766,27 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="75">
+      <c r="B4" s="91">
         <v>0.111</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="89" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="73" t="s">
-        <v>107</v>
+      <c r="D4" s="89" t="s">
+        <v>106</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="78"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="25" t="s">
         <v>70</v>
       </c>
@@ -2772,7 +2802,7 @@
         <v>69</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E6" s="28" t="s">
         <v>70</v>
@@ -2789,7 +2819,7 @@
         <v>69</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="28" t="s">
         <v>70</v>
@@ -2946,19 +2976,19 @@
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B17" s="46">
         <v>1</v>
       </c>
       <c r="C17" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="E17" s="48" t="s">
         <v>112</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -3002,18 +3032,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="79" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="A1" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="44" t="s">
         <v>46</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>6</v>
@@ -3033,10 +3063,10 @@
         <v>47</v>
       </c>
       <c r="B3" s="53" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" s="51"/>
       <c r="E3" s="49"/>
@@ -3049,10 +3079,10 @@
         <v>48</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="52"/>
@@ -3065,10 +3095,10 @@
         <v>49</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="49"/>
@@ -3081,10 +3111,10 @@
         <v>50</v>
       </c>
       <c r="B6" s="53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D6" s="49"/>
       <c r="E6" s="49"/>
@@ -3097,10 +3127,10 @@
         <v>51</v>
       </c>
       <c r="B7" s="53" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D7" s="49"/>
       <c r="E7" s="49"/>
@@ -3110,13 +3140,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="59"/>
     </row>
@@ -3125,7 +3155,7 @@
       <c r="B9" s="56"/>
       <c r="C9" s="56"/>
       <c r="D9" s="61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update groundtrack to plot different colors for ground stations
</commit_message>
<xml_diff>
--- a/docs/parameters.xlsx
+++ b/docs/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildesimoni/Desktop/EPFL/sem3/semester_project/digital_twin_CubeSat/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F9DA0A-ECC4-B248-B007-ED4EE71E9B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4CE398-4865-4A4C-AAB4-2388A906753C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,6 @@
     <t xml:space="preserve">Amount of energy received from the Sun for a given area. Taken as the Solar Constant (1 AU from the sun) </t>
   </si>
   <si>
-    <t>wikipedia page</t>
-  </si>
-  <si>
     <t>Wh</t>
   </si>
   <si>
@@ -148,30 +145,10 @@
 - Total energy: 7.2 V * 10.6 Ah = 76.32 Wh</t>
   </si>
   <si>
-    <t>Minimum battery energy to start an x-band communication session
-Calculated as: (mean_xband_consumption - mean_solar_input) * max_duration + min battery = (23.89 - 0.207) * 500/3600 + 15.264 = 18.55 Wh</t>
-  </si>
-  <si>
-    <t>Minimum battery energy to start a measurement session 
-Calculated as: (mean_measurement_consumption - mean_solar_input) * max_duration + min battery = (14.23 - 0.207) * 10560/3600 + 15.264) = 56.4 Wh
-(this simplification assumes that there is not data stored when the measurement window starts:  later, will be dynamically updated by checking data storage =&gt; might lower the measure threshold)</t>
-  </si>
-  <si>
-    <t>Minimum battery energy to start a uhf communication session
-Calculated as: (mean_uhf_consumption - mean_solar_input) * max_duration + min battery
-= (6.25 - 0.207) * 500/3600 + 15.264 = 16.10 Wh</t>
-  </si>
-  <si>
     <t>Mean solar input</t>
   </si>
   <si>
     <t>W</t>
-  </si>
-  <si>
-    <t>From previous student (GMAT simulation)</t>
-  </si>
-  <si>
-    <t>Including a safety factor of 0.9</t>
   </si>
   <si>
     <t>Number of solar panel cells</t>
@@ -194,9 +171,6 @@
   </si>
   <si>
     <t>Power System</t>
-  </si>
-  <si>
-    <t>Mean Consumption</t>
   </si>
   <si>
     <t>Subsystem</t>
@@ -643,12 +617,37 @@
       <t>) simulates a "randomly tumbling" satellite.</t>
     </r>
   </si>
+  <si>
+    <t>an introduction to solar radiation</t>
+  </si>
+  <si>
+    <t>Mean Consumption [W]</t>
+  </si>
+  <si>
+    <t>Simulation of 15 days with the current framework: got an average</t>
+  </si>
+  <si>
+    <t>Used to calculate the thresholds above with a margin of 0.5 =&gt; 3.615</t>
+  </si>
+  <si>
+    <t>Minimum battery energy to start a uhf communication session
+Calculated as: (mean_uhf_consumption - 0.5* mean_solar_input) * max_duration + min battery = (6.25 - 3.615) * 500/3600 + 15.264 = 15.63 Wh</t>
+  </si>
+  <si>
+    <t>Minimum battery energy to start an x-band communication session
+Calculated as: (mean_xband_consumption - mean_solar_input) * max_duration + min battery = (23.89 - 3.615) * 500/3600 + 15.264 = 18.08 Wh</t>
+  </si>
+  <si>
+    <t>Minimum battery energy to start a measurement session 
+Calculated as: (mean_measurement_consumption - mean_solar_input) * max_duration + min battery = (14.23 - 3.615) * 10560/3600 + 15.264) = 46.40 Wh
+(this simplification assumes that there is not data stored when the measurement window starts:  later, will be dynamically updated by checking data storage =&gt; might lower the measure threshold)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -768,6 +767,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1111,9 +1116,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1132,9 +1134,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1256,21 +1255,21 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1324,6 +1323,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1681,101 +1686,106 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="72"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
     </row>
     <row r="2" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="72"/>
-      <c r="B3" s="73"/>
-      <c r="C3" s="73"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="72"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="A8" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="72"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="71"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="71"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="77">
+      <c r="A14" s="70">
         <v>45611</v>
       </c>
-      <c r="B14" s="73"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="72"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
+      <c r="B15" s="71"/>
+      <c r="C15" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A12:C12"/>
@@ -1786,11 +1796,6 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1800,7 +1805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D47EFD6-0811-8141-81C1-0849D4B1537E}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1814,269 +1819,269 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="21">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="25">
+        <v>5.3</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="220" x14ac:dyDescent="0.2">
+      <c r="A6" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="B6" s="62">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="C6" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="63"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="65">
+        <v>6878</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="67">
+        <v>0</v>
+      </c>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="E8" s="80"/>
+    </row>
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="67">
+        <v>97.406499999999994</v>
+      </c>
+      <c r="C9" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="80"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="66" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="67">
+        <v>0</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E10" s="80"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="66" t="s">
+        <v>123</v>
+      </c>
+      <c r="B11" s="67">
+        <v>110</v>
+      </c>
+      <c r="C11" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" s="80"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="68" t="s">
+        <v>124</v>
+      </c>
+      <c r="B12" s="69">
+        <v>0</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="E12" s="81"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="B13" s="65">
+        <v>46.52</v>
+      </c>
+      <c r="C13" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="65"/>
+      <c r="E13" s="82" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B14" s="67">
+        <v>6.5650000000000004</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="67"/>
+      <c r="E14" s="83"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" s="69">
         <v>10</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B4" s="23">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="27">
-        <v>5.3</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="220" x14ac:dyDescent="0.2">
-      <c r="A6" s="63" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="64">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>105</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="65"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="66" t="s">
-        <v>126</v>
-      </c>
-      <c r="B7" s="67">
-        <v>6878</v>
-      </c>
-      <c r="C7" s="67" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="67" t="s">
-        <v>134</v>
-      </c>
-      <c r="E7" s="81" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="68" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="69">
-        <v>0</v>
-      </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69" t="s">
-        <v>137</v>
-      </c>
-      <c r="E8" s="82"/>
-    </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="69">
-        <v>97.406499999999994</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>136</v>
-      </c>
-      <c r="E9" s="82"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B10" s="69">
-        <v>0</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" s="69" t="s">
-        <v>135</v>
-      </c>
-      <c r="E10" s="82"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="68" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="69">
-        <v>110</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" s="69" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="82"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="70" t="s">
-        <v>131</v>
-      </c>
-      <c r="B12" s="71">
-        <v>0</v>
-      </c>
-      <c r="C12" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" s="83"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="66" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="67">
-        <v>46.52</v>
-      </c>
-      <c r="C13" s="67" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="84" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="69">
-        <v>6.5650000000000004</v>
-      </c>
-      <c r="C14" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="69"/>
-      <c r="E14" s="85"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="70" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="71">
-        <v>10</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="71"/>
-      <c r="E15" s="86"/>
+      <c r="C15" s="69" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="69"/>
+      <c r="E15" s="84"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="62"/>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="62"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="60"/>
+      <c r="C20" s="60"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="62"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="60"/>
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="60"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="62"/>
-      <c r="B22" s="62"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="60"/>
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="62"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2097,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C11073C-47B1-364A-8420-1F44036F49B1}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2111,44 +2116,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
+      <c r="A1" s="77" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3">
-        <v>1361</v>
+        <v>1367</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>14</v>
@@ -2156,164 +2161,164 @@
       <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="95" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="12">
+        <v>76.319999999999993</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="160" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="D5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="16"/>
+    </row>
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="13">
-        <v>76.319999999999993</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="B6" s="12">
+        <v>15.263999999999999</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="13">
-        <v>15.263999999999999</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>61.055999999999997</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>27</v>
+      <c r="E7" s="17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="13">
-        <v>56.4</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="A8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12">
+        <v>46.4</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="2">
+        <v>15.63</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="12">
+        <v>7.23</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E11" s="96" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="2">
-        <v>16.100000000000001</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="B12" s="12">
+        <v>28</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="16"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="13">
-        <v>18.55</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="31" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="B13" s="12">
+        <v>2.8354999999999999E-3</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="13">
-        <v>0.23</v>
-      </c>
-      <c r="C11" s="13" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="B14" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="16" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="13">
-        <v>28</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="13">
-        <v>2.8354999999999999E-3</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="13">
-        <v>0.25</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="18" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2321,7 +2326,7 @@
     <mergeCell ref="A1:E2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{3BAB174A-DD62-A348-8C87-58433BB670D5}"/>
+    <hyperlink ref="E4" r:id="rId1" location="v=onepage&amp;q=sollar%20irradiance%20constant%20variation&amp;f=false" xr:uid="{3BAB174A-DD62-A348-8C87-58433BB670D5}"/>
     <hyperlink ref="E13" r:id="rId2" xr:uid="{6CD05C9F-FE87-1940-84C6-F1F335E35C3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2333,7 +2338,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection sqref="A1:H2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2350,355 +2355,355 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="85" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="85"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-      <c r="F2" s="80"/>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="87" t="s">
+      <c r="G4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="87" t="s">
+      <c r="H4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87"/>
-      <c r="B4" s="87"/>
-      <c r="C4" s="6" t="s">
+      <c r="B5" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C5" s="33">
+        <v>1.6</v>
+      </c>
+      <c r="D5" s="34">
+        <v>1.6</v>
+      </c>
+      <c r="E5" s="34">
+        <v>1.6</v>
+      </c>
+      <c r="F5" s="34">
+        <v>1.6</v>
+      </c>
+      <c r="G5" s="34">
+        <v>1.6</v>
+      </c>
+      <c r="H5" s="35">
+        <v>1.6</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="B6" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="36">
+        <v>1.7</v>
+      </c>
+      <c r="D6" s="32">
+        <v>1.7</v>
+      </c>
+      <c r="E6" s="32">
+        <v>1.7</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1.7</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1.7</v>
+      </c>
+      <c r="H6" s="37">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="B7" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="C7" s="36">
+        <v>0.24</v>
+      </c>
+      <c r="D7" s="32">
+        <v>0.24</v>
+      </c>
+      <c r="E7" s="32">
+        <v>0.24</v>
+      </c>
+      <c r="F7" s="32">
+        <v>0.24</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0.24</v>
+      </c>
+      <c r="H7" s="37">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="B8" s="31">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="36">
+        <v>2.1</v>
+      </c>
+      <c r="D8" s="32">
+        <v>2.1</v>
+      </c>
+      <c r="E8" s="32">
+        <v>2.1</v>
+      </c>
+      <c r="F8" s="32">
+        <v>2.1</v>
+      </c>
+      <c r="G8" s="32">
+        <v>2.1</v>
+      </c>
+      <c r="H8" s="37">
+        <v>2.1</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="B9" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="C9" s="36">
+        <v>0</v>
+      </c>
+      <c r="D9" s="32">
+        <v>0</v>
+      </c>
+      <c r="E9" s="32">
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <v>0</v>
+      </c>
+      <c r="G9" s="32">
+        <v>17.64</v>
+      </c>
+      <c r="H9" s="37">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="B10" s="31">
+        <v>0.1</v>
+      </c>
+      <c r="C10" s="36">
+        <v>0.61</v>
+      </c>
+      <c r="D10" s="32">
+        <v>0</v>
+      </c>
+      <c r="E10" s="32">
+        <v>0.61</v>
+      </c>
+      <c r="F10" s="32">
+        <v>0.61</v>
+      </c>
+      <c r="G10" s="32">
+        <v>0.61</v>
+      </c>
+      <c r="H10" s="37">
+        <v>0.61</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="B11" s="31">
+        <v>0</v>
+      </c>
+      <c r="C11" s="36">
+        <v>0</v>
+      </c>
+      <c r="D11" s="32">
+        <v>0</v>
+      </c>
+      <c r="E11" s="32">
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <v>0</v>
+      </c>
+      <c r="G11" s="32">
+        <v>0</v>
+      </c>
+      <c r="H11" s="37">
+        <v>7.98</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C5" s="35">
-        <v>1.6</v>
-      </c>
-      <c r="D5" s="36">
-        <v>1.6</v>
-      </c>
-      <c r="E5" s="36">
-        <v>1.6</v>
-      </c>
-      <c r="F5" s="36">
-        <v>1.6</v>
-      </c>
-      <c r="G5" s="36">
-        <v>1.6</v>
-      </c>
-      <c r="H5" s="37">
-        <v>1.6</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="38">
-        <v>1.7</v>
-      </c>
-      <c r="D6" s="34">
-        <v>1.7</v>
-      </c>
-      <c r="E6" s="34">
-        <v>1.7</v>
-      </c>
-      <c r="F6" s="34">
-        <v>1.7</v>
-      </c>
-      <c r="G6" s="34">
-        <v>1.7</v>
-      </c>
-      <c r="H6" s="39">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="C7" s="38">
-        <v>0.24</v>
-      </c>
-      <c r="D7" s="34">
-        <v>0.24</v>
-      </c>
-      <c r="E7" s="34">
-        <v>0.24</v>
-      </c>
-      <c r="F7" s="34">
-        <v>0.24</v>
-      </c>
-      <c r="G7" s="34">
-        <v>0.24</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="C8" s="38">
-        <v>2.1</v>
-      </c>
-      <c r="D8" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="E8" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="F8" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="G8" s="34">
-        <v>2.1</v>
-      </c>
-      <c r="H8" s="39">
-        <v>2.1</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="33">
-        <v>0.2</v>
-      </c>
-      <c r="C9" s="38">
-        <v>0</v>
-      </c>
-      <c r="D9" s="34">
-        <v>0</v>
-      </c>
-      <c r="E9" s="34">
-        <v>0</v>
-      </c>
-      <c r="F9" s="34">
-        <v>0</v>
-      </c>
-      <c r="G9" s="34">
-        <v>17.64</v>
-      </c>
-      <c r="H9" s="39">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="33">
-        <v>0.1</v>
-      </c>
-      <c r="C10" s="38">
-        <v>0.61</v>
-      </c>
-      <c r="D10" s="34">
-        <v>0</v>
-      </c>
-      <c r="E10" s="34">
-        <v>0.61</v>
-      </c>
-      <c r="F10" s="34">
-        <v>0.61</v>
-      </c>
-      <c r="G10" s="34">
-        <v>0.61</v>
-      </c>
-      <c r="H10" s="39">
-        <v>0.61</v>
-      </c>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="33">
-        <v>0</v>
-      </c>
-      <c r="C11" s="38">
-        <v>0</v>
-      </c>
-      <c r="D11" s="34">
-        <v>0</v>
-      </c>
-      <c r="E11" s="34">
-        <v>0</v>
-      </c>
-      <c r="F11" s="34">
-        <v>0</v>
-      </c>
-      <c r="G11" s="34">
-        <v>0</v>
-      </c>
-      <c r="H11" s="39">
-        <v>7.98</v>
-      </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="40">
+      <c r="B12" s="86"/>
+      <c r="C12" s="38">
         <v>6.25</v>
       </c>
-      <c r="D12" s="41">
+      <c r="D12" s="39">
         <v>5.64</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="39">
         <v>6.25</v>
       </c>
-      <c r="F12" s="41">
+      <c r="F12" s="39">
         <v>6.25</v>
       </c>
-      <c r="G12" s="41">
+      <c r="G12" s="39">
         <v>23.89</v>
       </c>
-      <c r="H12" s="42">
+      <c r="H12" s="40">
         <v>14.23</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2733,262 +2738,262 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="77"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="91" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="89">
+        <v>0.111</v>
+      </c>
+      <c r="C4" s="87" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="92"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="79"/>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
-      <c r="D2" s="80"/>
-      <c r="E2" s="80"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="B6" s="25">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="28">
+        <v>6.6699999999999995E-5</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="25">
+        <v>2097152</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1.9199999999999998E-2</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="25">
         <v>10</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="93" t="s">
+      <c r="C10" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="25"/>
+      <c r="E10" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="91">
-        <v>0.111</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="89" t="s">
-        <v>106</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="94"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="B11" s="25">
+        <v>500</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="27">
-        <v>6.4999999999999997E-3</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="29" t="s">
+      <c r="D11" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B7" s="30">
-        <v>6.6699999999999995E-5</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B8" s="27">
-        <v>2097152</v>
-      </c>
-      <c r="C8" s="27" t="s">
+      <c r="E11" s="30"/>
+    </row>
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="25">
+        <v>10560</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="25">
+        <v>1500</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B9" s="31">
-        <v>1.9199999999999998E-2</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
+      <c r="E13" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B10" s="27">
-        <v>10</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
+      <c r="B14" s="25">
+        <v>1860</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="27">
-        <v>500</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="32"/>
-    </row>
-    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
+      <c r="E14" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="25">
+        <v>7200</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="25">
+        <v>15</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="27">
-        <v>10560</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="27">
-        <v>1500</v>
-      </c>
-      <c r="C13" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="27">
-        <v>1860</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="27">
-        <v>7200</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="27">
-        <v>15</v>
-      </c>
-      <c r="C16" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="46">
+      <c r="A17" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="44">
         <v>1</v>
       </c>
-      <c r="C17" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>111</v>
-      </c>
-      <c r="E17" s="48" t="s">
-        <v>112</v>
+      <c r="C17" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -3032,134 +3037,134 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="93" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="43" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+    </row>
+    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="49"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="47"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+    </row>
+    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="53" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="60" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-    </row>
-    <row r="3" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A3" s="55" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="53" t="s">
+      <c r="C6" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="57"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9" s="54"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="C3" s="32" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="51"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="55" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="53" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D4" s="49"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="53" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-    </row>
-    <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A6" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="55" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>119</v>
-      </c>
-      <c r="C8" s="58" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" s="59"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="61" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="50"/>
+      <c r="D22" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
update solar_power => solar_flux and correct minor type in excel doc
</commit_message>
<xml_diff>
--- a/docs/parameters.xlsx
+++ b/docs/parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathildesimoni/Desktop/EPFL/sem3/semester_project/digital_twin_CubeSat/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4CE398-4865-4A4C-AAB4-2388A906753C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCCB7A2-0EC0-E341-9615-BA73334CAE49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{24D85746-A0DA-644A-B01E-02F5A4C5B15B}"/>
   </bookViews>
@@ -630,10 +630,6 @@
     <t>Used to calculate the thresholds above with a margin of 0.5 =&gt; 3.615</t>
   </si>
   <si>
-    <t>Minimum battery energy to start a uhf communication session
-Calculated as: (mean_uhf_consumption - 0.5* mean_solar_input) * max_duration + min battery = (6.25 - 3.615) * 500/3600 + 15.264 = 15.63 Wh</t>
-  </si>
-  <si>
     <t>Minimum battery energy to start an x-band communication session
 Calculated as: (mean_xband_consumption - mean_solar_input) * max_duration + min battery = (23.89 - 3.615) * 500/3600 + 15.264 = 18.08 Wh</t>
   </si>
@@ -641,6 +637,10 @@
     <t>Minimum battery energy to start a measurement session 
 Calculated as: (mean_measurement_consumption - mean_solar_input) * max_duration + min battery = (14.23 - 3.615) * 10560/3600 + 15.264) = 46.40 Wh
 (this simplification assumes that there is not data stored when the measurement window starts:  later, will be dynamically updated by checking data storage =&gt; might lower the measure threshold)</t>
+  </si>
+  <si>
+    <t>Minimum battery energy to start a uhf communication session
+Calculated as: (mean_uhf_consumption - mean_solar_input) * max_duration + min battery = (6.25 - 3.615) * 500/3600 + 15.264 = 15.63 Wh</t>
   </si>
 </sst>
 </file>
@@ -1255,21 +1255,27 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1323,12 +1329,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1686,106 +1686,101 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="72"/>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
     </row>
     <row r="2" spans="1:3" ht="47" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="72"/>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
     </row>
     <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="72"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
     </row>
     <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
     </row>
     <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="72"/>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
     </row>
     <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="73" t="s">
+      <c r="A11" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="71"/>
-      <c r="C12" s="71"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="71"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
     </row>
     <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="70">
+      <c r="A14" s="77">
         <v>45611</v>
       </c>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="72"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="71"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="A12:C12"/>
@@ -1796,6 +1791,11 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1819,20 +1819,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -1909,7 +1909,7 @@
       <c r="D7" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="81" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1924,7 +1924,7 @@
       <c r="D8" s="67" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="80"/>
+      <c r="E8" s="82"/>
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="66" t="s">
@@ -1939,7 +1939,7 @@
       <c r="D9" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="80"/>
+      <c r="E9" s="82"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="66" t="s">
@@ -1954,7 +1954,7 @@
       <c r="D10" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="E10" s="80"/>
+      <c r="E10" s="82"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="66" t="s">
@@ -1969,7 +1969,7 @@
       <c r="D11" s="67" t="s">
         <v>128</v>
       </c>
-      <c r="E11" s="80"/>
+      <c r="E11" s="82"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="68" t="s">
@@ -1984,7 +1984,7 @@
       <c r="D12" s="69" t="s">
         <v>128</v>
       </c>
-      <c r="E12" s="81"/>
+      <c r="E12" s="83"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="64" t="s">
@@ -1997,7 +1997,7 @@
         <v>86</v>
       </c>
       <c r="D13" s="65"/>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="84" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2012,7 +2012,7 @@
         <v>86</v>
       </c>
       <c r="D14" s="67"/>
-      <c r="E14" s="83"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="68" t="s">
@@ -2025,7 +2025,7 @@
         <v>86</v>
       </c>
       <c r="D15" s="69"/>
-      <c r="E15" s="84"/>
+      <c r="E15" s="86"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="60"/>
@@ -2116,20 +2116,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -2161,7 +2161,7 @@
       <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="95" t="s">
+      <c r="E4" s="70" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2225,7 +2225,7 @@
         <v>17</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>35</v>
@@ -2242,7 +2242,7 @@
         <v>17</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>35</v>
@@ -2259,7 +2259,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="16" t="s">
         <v>35</v>
@@ -2278,7 +2278,7 @@
       <c r="D11" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E11" s="71" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2355,16 +2355,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
       <c r="I1" s="8" t="s">
         <v>54</v>
       </c>
@@ -2373,14 +2373,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
       <c r="I2" s="10" t="s">
         <v>56</v>
       </c>
@@ -2389,28 +2389,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="87" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="85"/>
-      <c r="B4" s="85"/>
+      <c r="A4" s="87"/>
+      <c r="B4" s="87"/>
       <c r="C4" s="5" t="s">
         <v>40</v>
       </c>
@@ -2629,10 +2629,10 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="85" t="s">
+      <c r="A12" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="86"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="38">
         <v>6.25</v>
       </c>
@@ -2738,20 +2738,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="77"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -2771,16 +2771,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="93" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="89">
+      <c r="B4" s="91">
         <v>0.111</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="D4" s="87" t="s">
+      <c r="D4" s="89" t="s">
         <v>99</v>
       </c>
       <c r="E4" s="19" t="s">
@@ -2788,10 +2788,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="92"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="92"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
       <c r="E5" s="23" t="s">
         <v>63</v>
       </c>
@@ -3037,11 +3037,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="42" t="s">

</xml_diff>